<commit_message>
Add gradlew wrapper files
</commit_message>
<xml_diff>
--- a/etc/WBS_TeamProject_Candy.xlsx
+++ b/etc/WBS_TeamProject_Candy.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\tjg_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\tjg_project\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A4C323-2594-4699-B2A2-78478A346D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF435BB-A51C-43CE-A169-D558BA51255B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4F68EF3D-DEC7-4864-A746-04C7E98A59CC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="142">
   <si>
     <t>프로젝트 명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1082,43 +1082,43 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="31" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="31" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1493,189 +1493,189 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="45"/>
-      <c r="F2" s="47" t="s">
+      <c r="D2" s="53"/>
+      <c r="F2" s="44" t="s">
         <v>105</v>
       </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
-      <c r="V2" s="48"/>
-      <c r="W2" s="48"/>
-      <c r="X2" s="48"/>
-      <c r="Y2" s="48"/>
-      <c r="Z2" s="48"/>
-      <c r="AA2" s="48"/>
-      <c r="AB2" s="48"/>
-      <c r="AC2" s="48"/>
-      <c r="AD2" s="48"/>
-      <c r="AE2" s="48"/>
-      <c r="AF2" s="48"/>
-      <c r="AG2" s="48"/>
-      <c r="AH2" s="48"/>
-      <c r="AI2" s="48"/>
-      <c r="AJ2" s="48"/>
-      <c r="AK2" s="48"/>
-      <c r="AL2" s="49"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="45"/>
+      <c r="V2" s="45"/>
+      <c r="W2" s="45"/>
+      <c r="X2" s="45"/>
+      <c r="Y2" s="45"/>
+      <c r="Z2" s="45"/>
+      <c r="AA2" s="45"/>
+      <c r="AB2" s="45"/>
+      <c r="AC2" s="45"/>
+      <c r="AD2" s="45"/>
+      <c r="AE2" s="45"/>
+      <c r="AF2" s="45"/>
+      <c r="AG2" s="45"/>
+      <c r="AH2" s="45"/>
+      <c r="AI2" s="45"/>
+      <c r="AJ2" s="45"/>
+      <c r="AK2" s="45"/>
+      <c r="AL2" s="46"/>
     </row>
     <row r="3" spans="2:103" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="56">
+      <c r="C3" s="54">
         <v>45945</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="51"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="51"/>
-      <c r="U3" s="51"/>
-      <c r="V3" s="51"/>
-      <c r="W3" s="51"/>
-      <c r="X3" s="51"/>
-      <c r="Y3" s="51"/>
-      <c r="Z3" s="51"/>
-      <c r="AA3" s="51"/>
-      <c r="AB3" s="51"/>
-      <c r="AC3" s="51"/>
-      <c r="AD3" s="51"/>
-      <c r="AE3" s="51"/>
-      <c r="AF3" s="51"/>
-      <c r="AG3" s="51"/>
-      <c r="AH3" s="51"/>
-      <c r="AI3" s="51"/>
-      <c r="AJ3" s="51"/>
-      <c r="AK3" s="51"/>
-      <c r="AL3" s="52"/>
+      <c r="D3" s="53"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="48"/>
+      <c r="V3" s="48"/>
+      <c r="W3" s="48"/>
+      <c r="X3" s="48"/>
+      <c r="Y3" s="48"/>
+      <c r="Z3" s="48"/>
+      <c r="AA3" s="48"/>
+      <c r="AB3" s="48"/>
+      <c r="AC3" s="48"/>
+      <c r="AD3" s="48"/>
+      <c r="AE3" s="48"/>
+      <c r="AF3" s="48"/>
+      <c r="AG3" s="48"/>
+      <c r="AH3" s="48"/>
+      <c r="AI3" s="48"/>
+      <c r="AJ3" s="48"/>
+      <c r="AK3" s="48"/>
+      <c r="AL3" s="49"/>
     </row>
     <row r="4" spans="2:103" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="56">
+      <c r="C4" s="54">
         <v>45992</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="51"/>
-      <c r="S4" s="51"/>
-      <c r="T4" s="51"/>
-      <c r="U4" s="51"/>
-      <c r="V4" s="51"/>
-      <c r="W4" s="51"/>
-      <c r="X4" s="51"/>
-      <c r="Y4" s="51"/>
-      <c r="Z4" s="51"/>
-      <c r="AA4" s="51"/>
-      <c r="AB4" s="51"/>
-      <c r="AC4" s="51"/>
-      <c r="AD4" s="51"/>
-      <c r="AE4" s="51"/>
-      <c r="AF4" s="51"/>
-      <c r="AG4" s="51"/>
-      <c r="AH4" s="51"/>
-      <c r="AI4" s="51"/>
-      <c r="AJ4" s="51"/>
-      <c r="AK4" s="51"/>
-      <c r="AL4" s="52"/>
+      <c r="D4" s="53"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="48"/>
+      <c r="U4" s="48"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="48"/>
+      <c r="Y4" s="48"/>
+      <c r="Z4" s="48"/>
+      <c r="AA4" s="48"/>
+      <c r="AB4" s="48"/>
+      <c r="AC4" s="48"/>
+      <c r="AD4" s="48"/>
+      <c r="AE4" s="48"/>
+      <c r="AF4" s="48"/>
+      <c r="AG4" s="48"/>
+      <c r="AH4" s="48"/>
+      <c r="AI4" s="48"/>
+      <c r="AJ4" s="48"/>
+      <c r="AK4" s="48"/>
+      <c r="AL4" s="49"/>
     </row>
     <row r="5" spans="2:103" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="45"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54"/>
-      <c r="M5" s="54"/>
-      <c r="N5" s="54"/>
-      <c r="O5" s="54"/>
-      <c r="P5" s="54"/>
-      <c r="Q5" s="54"/>
-      <c r="R5" s="54"/>
-      <c r="S5" s="54"/>
-      <c r="T5" s="54"/>
-      <c r="U5" s="54"/>
-      <c r="V5" s="54"/>
-      <c r="W5" s="54"/>
-      <c r="X5" s="54"/>
-      <c r="Y5" s="54"/>
-      <c r="Z5" s="54"/>
-      <c r="AA5" s="54"/>
-      <c r="AB5" s="54"/>
-      <c r="AC5" s="54"/>
-      <c r="AD5" s="54"/>
-      <c r="AE5" s="54"/>
-      <c r="AF5" s="54"/>
-      <c r="AG5" s="54"/>
-      <c r="AH5" s="54"/>
-      <c r="AI5" s="54"/>
-      <c r="AJ5" s="54"/>
-      <c r="AK5" s="54"/>
-      <c r="AL5" s="55"/>
+      <c r="D5" s="53"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="51"/>
+      <c r="R5" s="51"/>
+      <c r="S5" s="51"/>
+      <c r="T5" s="51"/>
+      <c r="U5" s="51"/>
+      <c r="V5" s="51"/>
+      <c r="W5" s="51"/>
+      <c r="X5" s="51"/>
+      <c r="Y5" s="51"/>
+      <c r="Z5" s="51"/>
+      <c r="AA5" s="51"/>
+      <c r="AB5" s="51"/>
+      <c r="AC5" s="51"/>
+      <c r="AD5" s="51"/>
+      <c r="AE5" s="51"/>
+      <c r="AF5" s="51"/>
+      <c r="AG5" s="51"/>
+      <c r="AH5" s="51"/>
+      <c r="AI5" s="51"/>
+      <c r="AJ5" s="51"/>
+      <c r="AK5" s="51"/>
+      <c r="AL5" s="52"/>
     </row>
     <row r="6" spans="2:103" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="44">
+      <c r="C6" s="55">
         <v>45958</v>
       </c>
-      <c r="D6" s="45"/>
+      <c r="D6" s="53"/>
     </row>
     <row r="7" spans="2:103" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="45"/>
+      <c r="D7" s="53"/>
     </row>
     <row r="10" spans="2:103" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="25"/>
@@ -1690,104 +1690,104 @@
       <c r="K10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L10" s="46" t="s">
+      <c r="L10" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="M10" s="46"/>
-      <c r="N10" s="46"/>
-      <c r="O10" s="46"/>
-      <c r="P10" s="46"/>
-      <c r="Q10" s="46"/>
-      <c r="R10" s="46"/>
-      <c r="S10" s="46"/>
-      <c r="T10" s="46"/>
-      <c r="U10" s="46"/>
-      <c r="V10" s="46"/>
-      <c r="W10" s="46"/>
-      <c r="X10" s="46"/>
-      <c r="Y10" s="46"/>
-      <c r="Z10" s="46"/>
-      <c r="AA10" s="46"/>
-      <c r="AB10" s="46"/>
-      <c r="AC10" s="46"/>
-      <c r="AD10" s="46"/>
-      <c r="AE10" s="46"/>
-      <c r="AF10" s="46"/>
-      <c r="AG10" s="46"/>
-      <c r="AH10" s="46"/>
-      <c r="AI10" s="46"/>
-      <c r="AJ10" s="46"/>
-      <c r="AK10" s="46"/>
-      <c r="AL10" s="46"/>
-      <c r="AM10" s="46"/>
-      <c r="AN10" s="46"/>
-      <c r="AO10" s="46"/>
-      <c r="AP10" s="46"/>
-      <c r="AQ10" s="46" t="s">
+      <c r="M10" s="56"/>
+      <c r="N10" s="56"/>
+      <c r="O10" s="56"/>
+      <c r="P10" s="56"/>
+      <c r="Q10" s="56"/>
+      <c r="R10" s="56"/>
+      <c r="S10" s="56"/>
+      <c r="T10" s="56"/>
+      <c r="U10" s="56"/>
+      <c r="V10" s="56"/>
+      <c r="W10" s="56"/>
+      <c r="X10" s="56"/>
+      <c r="Y10" s="56"/>
+      <c r="Z10" s="56"/>
+      <c r="AA10" s="56"/>
+      <c r="AB10" s="56"/>
+      <c r="AC10" s="56"/>
+      <c r="AD10" s="56"/>
+      <c r="AE10" s="56"/>
+      <c r="AF10" s="56"/>
+      <c r="AG10" s="56"/>
+      <c r="AH10" s="56"/>
+      <c r="AI10" s="56"/>
+      <c r="AJ10" s="56"/>
+      <c r="AK10" s="56"/>
+      <c r="AL10" s="56"/>
+      <c r="AM10" s="56"/>
+      <c r="AN10" s="56"/>
+      <c r="AO10" s="56"/>
+      <c r="AP10" s="56"/>
+      <c r="AQ10" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="AR10" s="46"/>
-      <c r="AS10" s="46"/>
-      <c r="AT10" s="46"/>
-      <c r="AU10" s="46"/>
-      <c r="AV10" s="46"/>
-      <c r="AW10" s="46"/>
-      <c r="AX10" s="46"/>
-      <c r="AY10" s="46"/>
-      <c r="AZ10" s="46"/>
-      <c r="BA10" s="46"/>
-      <c r="BB10" s="46"/>
-      <c r="BC10" s="46"/>
-      <c r="BD10" s="46"/>
-      <c r="BE10" s="46"/>
-      <c r="BF10" s="46"/>
-      <c r="BG10" s="46"/>
-      <c r="BH10" s="46"/>
-      <c r="BI10" s="46"/>
-      <c r="BJ10" s="46"/>
-      <c r="BK10" s="46"/>
-      <c r="BL10" s="46"/>
-      <c r="BM10" s="46"/>
-      <c r="BN10" s="46"/>
-      <c r="BO10" s="46"/>
-      <c r="BP10" s="46"/>
-      <c r="BQ10" s="46"/>
-      <c r="BR10" s="46"/>
-      <c r="BS10" s="46"/>
-      <c r="BT10" s="46"/>
-      <c r="BU10" s="46" t="s">
+      <c r="AR10" s="56"/>
+      <c r="AS10" s="56"/>
+      <c r="AT10" s="56"/>
+      <c r="AU10" s="56"/>
+      <c r="AV10" s="56"/>
+      <c r="AW10" s="56"/>
+      <c r="AX10" s="56"/>
+      <c r="AY10" s="56"/>
+      <c r="AZ10" s="56"/>
+      <c r="BA10" s="56"/>
+      <c r="BB10" s="56"/>
+      <c r="BC10" s="56"/>
+      <c r="BD10" s="56"/>
+      <c r="BE10" s="56"/>
+      <c r="BF10" s="56"/>
+      <c r="BG10" s="56"/>
+      <c r="BH10" s="56"/>
+      <c r="BI10" s="56"/>
+      <c r="BJ10" s="56"/>
+      <c r="BK10" s="56"/>
+      <c r="BL10" s="56"/>
+      <c r="BM10" s="56"/>
+      <c r="BN10" s="56"/>
+      <c r="BO10" s="56"/>
+      <c r="BP10" s="56"/>
+      <c r="BQ10" s="56"/>
+      <c r="BR10" s="56"/>
+      <c r="BS10" s="56"/>
+      <c r="BT10" s="56"/>
+      <c r="BU10" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="BV10" s="46"/>
-      <c r="BW10" s="46"/>
-      <c r="BX10" s="46"/>
-      <c r="BY10" s="46"/>
-      <c r="BZ10" s="46"/>
-      <c r="CA10" s="46"/>
-      <c r="CB10" s="46"/>
-      <c r="CC10" s="46"/>
-      <c r="CD10" s="46"/>
-      <c r="CE10" s="46"/>
-      <c r="CF10" s="46"/>
-      <c r="CG10" s="46"/>
-      <c r="CH10" s="46"/>
-      <c r="CI10" s="46"/>
-      <c r="CJ10" s="46"/>
-      <c r="CK10" s="46"/>
-      <c r="CL10" s="46"/>
-      <c r="CM10" s="46"/>
-      <c r="CN10" s="46"/>
-      <c r="CO10" s="46"/>
-      <c r="CP10" s="46"/>
-      <c r="CQ10" s="46"/>
-      <c r="CR10" s="46"/>
-      <c r="CS10" s="46"/>
-      <c r="CT10" s="46"/>
-      <c r="CU10" s="46"/>
-      <c r="CV10" s="46"/>
-      <c r="CW10" s="46"/>
-      <c r="CX10" s="46"/>
-      <c r="CY10" s="46"/>
+      <c r="BV10" s="56"/>
+      <c r="BW10" s="56"/>
+      <c r="BX10" s="56"/>
+      <c r="BY10" s="56"/>
+      <c r="BZ10" s="56"/>
+      <c r="CA10" s="56"/>
+      <c r="CB10" s="56"/>
+      <c r="CC10" s="56"/>
+      <c r="CD10" s="56"/>
+      <c r="CE10" s="56"/>
+      <c r="CF10" s="56"/>
+      <c r="CG10" s="56"/>
+      <c r="CH10" s="56"/>
+      <c r="CI10" s="56"/>
+      <c r="CJ10" s="56"/>
+      <c r="CK10" s="56"/>
+      <c r="CL10" s="56"/>
+      <c r="CM10" s="56"/>
+      <c r="CN10" s="56"/>
+      <c r="CO10" s="56"/>
+      <c r="CP10" s="56"/>
+      <c r="CQ10" s="56"/>
+      <c r="CR10" s="56"/>
+      <c r="CS10" s="56"/>
+      <c r="CT10" s="56"/>
+      <c r="CU10" s="56"/>
+      <c r="CV10" s="56"/>
+      <c r="CW10" s="56"/>
+      <c r="CX10" s="56"/>
+      <c r="CY10" s="56"/>
     </row>
     <row r="11" spans="2:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="26"/>
@@ -3771,13 +3771,27 @@
         <v>62</v>
       </c>
       <c r="E49" s="11"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="24"/>
-      <c r="H49" s="24"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="10"/>
+      <c r="F49" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G49" s="24">
+        <v>45971</v>
+      </c>
+      <c r="H49" s="24">
+        <v>45974</v>
+      </c>
+      <c r="I49" s="9">
+        <v>1</v>
+      </c>
+      <c r="J49" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="K49" s="12"/>
       <c r="L49" s="38"/>
+      <c r="AZ49" s="32"/>
+      <c r="BA49" s="32"/>
+      <c r="BB49" s="32"/>
+      <c r="BC49" s="32"/>
       <c r="BZ49" s="5"/>
       <c r="CA49" s="5"/>
       <c r="CG49" s="5"/>
@@ -3801,13 +3815,27 @@
       <c r="E50" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F50" s="6"/>
-      <c r="G50" s="24"/>
-      <c r="H50" s="24"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="10"/>
+      <c r="F50" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G50" s="24">
+        <v>45971</v>
+      </c>
+      <c r="H50" s="24">
+        <v>45974</v>
+      </c>
+      <c r="I50" s="9">
+        <v>1</v>
+      </c>
+      <c r="J50" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="K50" s="12"/>
       <c r="L50" s="38"/>
+      <c r="AZ50" s="32"/>
+      <c r="BA50" s="32"/>
+      <c r="BB50" s="32"/>
+      <c r="BC50" s="32"/>
       <c r="BZ50" s="5"/>
       <c r="CA50" s="5"/>
       <c r="CG50" s="5"/>
@@ -3831,13 +3859,27 @@
       <c r="E51" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="F51" s="6"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="9"/>
-      <c r="J51" s="10"/>
+      <c r="F51" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G51" s="24">
+        <v>45971</v>
+      </c>
+      <c r="H51" s="24">
+        <v>45974</v>
+      </c>
+      <c r="I51" s="9">
+        <v>1</v>
+      </c>
+      <c r="J51" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="K51" s="12"/>
       <c r="L51" s="38"/>
+      <c r="AZ51" s="32"/>
+      <c r="BA51" s="32"/>
+      <c r="BB51" s="32"/>
+      <c r="BC51" s="32"/>
       <c r="BZ51" s="5"/>
       <c r="CA51" s="5"/>
       <c r="CG51" s="5"/>
@@ -3861,13 +3903,27 @@
       <c r="E52" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="F52" s="6"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="24"/>
-      <c r="I52" s="9"/>
-      <c r="J52" s="10"/>
+      <c r="F52" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G52" s="24">
+        <v>45971</v>
+      </c>
+      <c r="H52" s="24">
+        <v>45974</v>
+      </c>
+      <c r="I52" s="9">
+        <v>1</v>
+      </c>
+      <c r="J52" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="K52" s="12"/>
       <c r="L52" s="38"/>
+      <c r="AZ52" s="32"/>
+      <c r="BA52" s="32"/>
+      <c r="BB52" s="32"/>
+      <c r="BC52" s="32"/>
       <c r="BZ52" s="5"/>
       <c r="CA52" s="5"/>
       <c r="CG52" s="5"/>
@@ -3891,13 +3947,27 @@
       <c r="E53" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="F53" s="6"/>
-      <c r="G53" s="24"/>
-      <c r="H53" s="24"/>
-      <c r="I53" s="9"/>
-      <c r="J53" s="10"/>
+      <c r="F53" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G53" s="24">
+        <v>45971</v>
+      </c>
+      <c r="H53" s="24">
+        <v>45974</v>
+      </c>
+      <c r="I53" s="9">
+        <v>1</v>
+      </c>
+      <c r="J53" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="K53" s="12"/>
       <c r="L53" s="38"/>
+      <c r="AZ53" s="32"/>
+      <c r="BA53" s="32"/>
+      <c r="BB53" s="32"/>
+      <c r="BC53" s="32"/>
       <c r="BZ53" s="5"/>
       <c r="CA53" s="5"/>
       <c r="CG53" s="5"/>
@@ -4334,16 +4404,16 @@
   <autoFilter ref="B12:K12" xr:uid="{5F753AA6-DE5C-49F2-BB7C-CC2DC561C87B}"/>
   <dataConsolidate/>
   <mergeCells count="10">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="BU10:CY10"/>
+    <mergeCell ref="L10:AP10"/>
+    <mergeCell ref="AQ10:BT10"/>
     <mergeCell ref="F2:AL5"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="BU10:CY10"/>
-    <mergeCell ref="L10:AP10"/>
-    <mergeCell ref="AQ10:BT10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="F13:F25 F26:H65">

</xml_diff>